<commit_message>
Modificaciones en modulos de transacciones en SAP
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eny_t\Documents\UiPath\Cyborg_Bajas\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B367BA5-5BBD-4744-9F16-4309F0DF34C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E65D49B-414C-4DB2-9B73-099457BD8126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="-120" windowWidth="19710" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -228,55 +228,55 @@
     <t>Contraseña</t>
   </si>
   <si>
+    <t>Lenguaje</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>Nombre de la conexión de SAP (ambiente)</t>
+  </si>
+  <si>
+    <t>Usuario de inicio de sesión en SAP</t>
+  </si>
+  <si>
+    <t>Tabla Empleado en SAP</t>
+  </si>
+  <si>
+    <t>TablaEmpleado</t>
+  </si>
+  <si>
+    <t>PA0105</t>
+  </si>
+  <si>
+    <t>Nombre de la tabla del empleado en SAP</t>
+  </si>
+  <si>
+    <t>Transacciones en SAP</t>
+  </si>
+  <si>
+    <t>TransaccionSE16N</t>
+  </si>
+  <si>
+    <t>SE16N</t>
+  </si>
+  <si>
+    <t>Transacción para ingresar tabla del empleado</t>
+  </si>
+  <si>
+    <t>TransaccionSU01</t>
+  </si>
+  <si>
+    <t>SU01</t>
+  </si>
+  <si>
+    <t>Transacción para modificar el usuario en SAP</t>
+  </si>
+  <si>
+    <t>ProcessABCQueue</t>
+  </si>
+  <si>
     <t>Sopaconsal7</t>
-  </si>
-  <si>
-    <t>Lenguaje</t>
-  </si>
-  <si>
-    <t>ES</t>
-  </si>
-  <si>
-    <t>Nombre de la conexión de SAP (ambiente)</t>
-  </si>
-  <si>
-    <t>Usuario de inicio de sesión en SAP</t>
-  </si>
-  <si>
-    <t>Tabla Empleado en SAP</t>
-  </si>
-  <si>
-    <t>TablaEmpleado</t>
-  </si>
-  <si>
-    <t>PA0105</t>
-  </si>
-  <si>
-    <t>Nombre de la tabla del empleado en SAP</t>
-  </si>
-  <si>
-    <t>Transacciones en SAP</t>
-  </si>
-  <si>
-    <t>TransaccionSE16N</t>
-  </si>
-  <si>
-    <t>SE16N</t>
-  </si>
-  <si>
-    <t>Transacción para ingresar tabla del empleado</t>
-  </si>
-  <si>
-    <t>TransaccionSU01</t>
-  </si>
-  <si>
-    <t>SU01</t>
-  </si>
-  <si>
-    <t>Transacción para modificar el usuario en SAP</t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
   </si>
 </sst>
 </file>
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -713,7 +713,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -819,7 +819,7 @@
         <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
@@ -841,7 +841,7 @@
         <v>65</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
@@ -849,7 +849,7 @@
         <v>66</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
         <v>66</v>
@@ -857,60 +857,60 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s">
         <v>68</v>
       </c>
-      <c r="B19" t="s">
-        <v>69</v>
-      </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" t="s">
         <v>73</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>74</v>
-      </c>
-      <c r="C21" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" t="s">
         <v>77</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>78</v>
-      </c>
-      <c r="C23" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
         <v>80</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>81</v>
-      </c>
-      <c r="C24" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
V 1.1.1 Se han modificado los módulos Outlook e IniciarSesionSap. Se añadieron correcciones para QA, (BP) y validación de errores (Testing)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eny_t\Documents\UiPath\Cyborg_Bajas\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E65D49B-414C-4DB2-9B73-099457BD8126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1FF49B-2FE2-440E-9A30-1A047C14E489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="-120" windowWidth="19710" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -277,6 +277,21 @@
   </si>
   <si>
     <t>Sopaconsal7</t>
+  </si>
+  <si>
+    <t>euunice3@gmail.com</t>
+  </si>
+  <si>
+    <t>Correo al que se le envía notificación en caso de no haber correo nuevo de RH</t>
+  </si>
+  <si>
+    <t>ToInicioSAP</t>
+  </si>
+  <si>
+    <t>Correo al que se le envía notificación en caso de no haber podido iniciar sesión en SAP</t>
+  </si>
+  <si>
+    <t>ToCorreoNuevo</t>
   </si>
 </sst>
 </file>
@@ -660,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -805,116 +820,136 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="A14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" t="s">
-        <v>69</v>
-      </c>
+      <c r="A15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16">
-        <v>350</v>
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
+        <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="B17">
+        <v>350</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A20" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>80</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1887,6 +1922,8 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
V 1.1.1 Se añadieron correcciones para QA, limpieza de código (BP) y validación de errores (Testing)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eny_t\Documents\UiPath\Cyborg_Bajas\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1FF49B-2FE2-440E-9A30-1A047C14E489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0E4681-6895-4832-9177-849B1646FAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="-120" windowWidth="19710" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="92">
   <si>
     <t>Name</t>
   </si>
@@ -292,6 +292,15 @@
   </si>
   <si>
     <t>ToCorreoNuevo</t>
+  </si>
+  <si>
+    <t>LogonPath</t>
+  </si>
+  <si>
+    <t>C:\Program Files (x86)\SAP\FrontEnd\SAPgui\saplogon.exe</t>
+  </si>
+  <si>
+    <t>Ruta de la aplicación SAP</t>
   </si>
 </sst>
 </file>
@@ -675,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -838,119 +847,129 @@
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" t="s">
-        <v>69</v>
+      <c r="A16" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17">
-        <v>350</v>
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="B18">
+        <v>350</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B20" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A22" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
+      <c r="A22" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A23" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" t="s">
-        <v>74</v>
-      </c>
+      <c r="A23" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A24" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
+      <c r="A24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C25" t="s">
-        <v>78</v>
-      </c>
+      <c r="A25" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A26" s="6" t="s">
+      <c r="A26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>80</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1924,6 +1943,7 @@
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>